<commit_message>
Collected 7 data points
</commit_message>
<xml_diff>
--- a/533DataAnalysis.xlsx
+++ b/533DataAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedRo\OneDrive\Documents\Academic Texts\COOOOOOODE\GitPages\533-GithubProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08EAA0EA-81A9-4067-BC35-3FF92E16E9A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC2DCFC-9692-46FE-AF9E-37AF36AAD1AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9AF25E2E-0873-4E84-98FB-C0D304ECB5FA}"/>
   </bookViews>
@@ -31,6 +31,59 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+  <si>
+    <t>User/Repository</t>
+  </si>
+  <si>
+    <t># of Commits</t>
+  </si>
+  <si>
+    <t># of Contributors</t>
+  </si>
+  <si>
+    <t># of Lurkers</t>
+  </si>
+  <si>
+    <t>Repo File Size (KB)</t>
+  </si>
+  <si>
+    <t># of Releases</t>
+  </si>
+  <si>
+    <t>GhostPack/Seatbelt</t>
+  </si>
+  <si>
+    <t>discordjs/discord.js</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>davidojoy/BetterJoy</t>
+  </si>
+  <si>
+    <t>Avg. Time Between Commits (H)</t>
+  </si>
+  <si>
+    <t>Avg. Time Between Releases (D)</t>
+  </si>
+  <si>
+    <t>citra-emu/citra</t>
+  </si>
+  <si>
+    <t>apache/druid</t>
+  </si>
+  <si>
+    <t>apache/dubbo</t>
+  </si>
+  <si>
+    <t>apache/cayenne</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,12 +433,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC89DFE2-D99A-4FD9-A630-7BE2F52AF55D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" customWidth="1"/>
+    <col min="8" max="8" width="26.77734375" customWidth="1"/>
+    <col min="9" max="11" width="8.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>186</v>
+      </c>
+      <c r="C2">
+        <v>124</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>940</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>4970</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>269</v>
+      </c>
+      <c r="E3">
+        <v>263</v>
+      </c>
+      <c r="F3">
+        <v>71800</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>231</v>
+      </c>
+      <c r="C4">
+        <v>117</v>
+      </c>
+      <c r="D4">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>15204</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>8971</v>
+      </c>
+      <c r="C5">
+        <v>7.4160000000000004</v>
+      </c>
+      <c r="D5">
+        <v>198</v>
+      </c>
+      <c r="E5">
+        <v>187</v>
+      </c>
+      <c r="F5">
+        <v>68564</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>10907</v>
+      </c>
+      <c r="C6">
+        <v>6.7830000000000004</v>
+      </c>
+      <c r="D6">
+        <v>363</v>
+      </c>
+      <c r="E6">
+        <v>353</v>
+      </c>
+      <c r="F6">
+        <v>226126</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>4602</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>369</v>
+      </c>
+      <c r="E7">
+        <v>362</v>
+      </c>
+      <c r="F7">
+        <v>30969</v>
+      </c>
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>78.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>667</v>
+      </c>
+      <c r="C8">
+        <v>18.616</v>
+      </c>
+      <c r="D8">
+        <v>33</v>
+      </c>
+      <c r="E8">
+        <v>31</v>
+      </c>
+      <c r="F8">
+        <v>88954</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>